<commit_message>
implémentation jsp et action de gestion de prêt
</commit_message>
<xml_diff>
--- a/ActionsStruts.xlsx
+++ b/ActionsStruts.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$42</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="170">
   <si>
     <t>jsp</t>
   </si>
@@ -649,17 +649,10 @@
     <t>Ajouter un exemplaire de topo</t>
   </si>
   <si>
-    <t>Accéder à la page d'ajout d'un exemplaire de topo</t>
-  </si>
-  <si>
     <t>ajouterExemplaire.jsp</t>
   </si>
   <si>
     <t>INPUT : ajouterExemplaire.jsp</t>
-  </si>
-  <si>
-    <t>SUCCESS : redirectAction / infoUtilisateur
-INPUT (si aucune correspondance dans la base de données) : ajouterExemplaire.jsp</t>
   </si>
   <si>
     <t>Element du formulaire</t>
@@ -677,33 +670,6 @@
     <t>infoExemplaireTopo.jsp</t>
   </si>
   <si>
-    <t>ExemplaireTopo exemplaire</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Session</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : Utilisateur utilisateur
-Element du formulaire</t>
-    </r>
-  </si>
-  <si>
     <t>redirectAction / infoExemplaireTopo</t>
   </si>
   <si>
@@ -728,9 +694,6 @@
     <t>String titreTopo
 Date debut
 Date fin</t>
-  </si>
-  <si>
-    <t>Afficher la liste des exemplaires du topo dispo aux dates souhaités</t>
   </si>
   <si>
     <t>EmprunterAction / emprunter</t>
@@ -766,6 +729,85 @@
   </si>
   <si>
     <t>List&lt;ExemplaireTopo&gt; listExemplaire</t>
+  </si>
+  <si>
+    <t>InfoExemplaireAction / versInfo</t>
+  </si>
+  <si>
+    <t>ExemplaireTopo exemplaire
+List&lt;Emprunt&gt; listEmprunt</t>
+  </si>
+  <si>
+    <t>int empruntId
+int exemplaireId</t>
+  </si>
+  <si>
+    <t>Accéder à la page d'ajout d'un exemplaire de ce topo</t>
+  </si>
+  <si>
+    <t>AjouterExemplaireAction / ajouter</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">String titreTopo
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Utilisateur utilisateur</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">String titreTopo
+String titre
+String texte
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Session</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Utilisateur utilisateur</t>
+    </r>
+  </si>
+  <si>
+    <t>SUCCESS : redirectAction / infoUtilisateur</t>
+  </si>
+  <si>
+    <t>Afficher la liste des exemplaires du topo disponibles aux dates souhaités</t>
   </si>
 </sst>
 </file>
@@ -814,7 +856,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -842,12 +884,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -922,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -978,7 +1014,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1275,11 +1320,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="107" defaultRowHeight="15"/>
@@ -1394,7 +1439,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1418,7 +1463,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="11"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1440,7 +1485,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="11"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1462,7 +1507,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="11"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1484,7 +1529,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="11"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1508,7 +1553,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
-      <c r="A10" s="11"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1530,7 +1575,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="11"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1554,7 +1599,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="11"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1576,7 +1621,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="75">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1602,7 +1647,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="60">
-      <c r="A14" s="11"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
@@ -1624,7 +1669,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="11"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1646,7 +1691,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="11"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -1668,7 +1713,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="75">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1694,7 +1739,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30">
-      <c r="A18" s="11"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
@@ -1718,7 +1763,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="90">
-      <c r="A19" s="11"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
@@ -1742,7 +1787,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
-      <c r="A20" s="11"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
@@ -1766,7 +1811,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="11"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
@@ -1840,7 +1885,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1864,8 +1909,8 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="30">
-      <c r="A25" s="11"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="19"/>
+      <c r="B25" s="15" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -1889,7 +1934,7 @@
       <c r="A26" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -1958,19 +2003,19 @@
     <row r="29" spans="1:8" ht="45">
       <c r="A29" s="17"/>
       <c r="B29" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>41</v>
@@ -1980,7 +2025,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="60">
-      <c r="A30" s="18"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="4" t="s">
         <v>140</v>
       </c>
@@ -1988,288 +2033,317 @@
         <v>141</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="75">
-      <c r="A31" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>72</v>
+    <row r="31" spans="1:8" ht="30">
+      <c r="A31" s="18"/>
+      <c r="B31" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>69</v>
+        <v>164</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="H31" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="75">
-      <c r="A32" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>74</v>
+      <c r="A32" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F32" s="5" t="s">
         <v>69</v>
       </c>
       <c r="G32" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="75">
+      <c r="A33" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="H32" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="75">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:8" ht="75">
+      <c r="A34" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E34" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="F34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="1:8" ht="90">
-      <c r="A34" s="9" t="s">
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="1:8" ht="90">
+      <c r="A35" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C35" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E35" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="1:8" ht="90">
-      <c r="A35" s="11" t="s">
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="1:8" ht="90">
+      <c r="A36" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B36" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C36" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35" s="10" t="s">
+      <c r="D36" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="30">
-      <c r="A36" s="11"/>
-      <c r="B36" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>157</v>
-      </c>
       <c r="F36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H36" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="11"/>
+    <row r="37" spans="1:8" ht="30">
+      <c r="A37" s="22"/>
       <c r="B37" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="22"/>
+      <c r="B38" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E38" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="1:8" ht="30">
-      <c r="A38" s="11"/>
-      <c r="B38" s="9" t="s">
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" ht="30">
+      <c r="A39" s="22"/>
+      <c r="B39" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="10" t="s">
+      <c r="D39" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="30">
-      <c r="A39" s="11"/>
-      <c r="B39" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>146</v>
+      <c r="F39" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="H39" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="90">
-      <c r="A40" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" s="9" t="s">
+    <row r="40" spans="1:8" ht="60">
+      <c r="A40" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="14" t="s">
-        <v>153</v>
+      <c r="D40" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>167</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>156</v>
+      <c r="D41" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F41" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>154</v>
+        <v>121</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>150</v>
       </c>
       <c r="H41" s="9" t="s">
         <v>125</v>
       </c>
     </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="21"/>
+      <c r="B42" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H42" s="3"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H41"/>
-  <mergeCells count="6">
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="A35:A39"/>
+  <autoFilter ref="A1:H42"/>
+  <mergeCells count="7">
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A36:A39"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A5:A12"/>

</xml_diff>

<commit_message>
correction bugs et mise en page
</commit_message>
<xml_diff>
--- a/ActionsStruts.xlsx
+++ b/ActionsStruts.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$41</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="170">
   <si>
     <t>jsp</t>
   </si>
@@ -1005,6 +1005,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1014,16 +1020,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1320,11 +1320,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="107" defaultRowHeight="15"/>
@@ -1439,7 +1439,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1463,7 +1463,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1507,7 +1507,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1529,7 +1529,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
-      <c r="A10" s="19"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="19"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="19"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1621,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="75">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1647,7 +1647,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="60">
-      <c r="A14" s="19"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1669,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="19"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1691,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="19"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -1713,7 +1713,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="75">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30">
-      <c r="A18" s="19"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
@@ -1763,7 +1763,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="90">
-      <c r="A19" s="19"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
@@ -1787,7 +1787,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
-      <c r="A20" s="19"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
@@ -1811,7 +1811,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="19"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
@@ -1885,7 +1885,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1909,7 +1909,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="30">
-      <c r="A25" s="19"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="15" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="18" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -1955,7 +1955,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="17"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="4" t="s">
         <v>75</v>
       </c>
@@ -1979,7 +1979,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30">
-      <c r="A28" s="17"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -2001,7 +2001,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="45">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4" t="s">
         <v>155</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="60">
-      <c r="A30" s="17"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4" t="s">
         <v>140</v>
       </c>
@@ -2049,7 +2049,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="30">
-      <c r="A31" s="18"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="4" t="s">
         <v>142</v>
       </c>
@@ -2169,7 +2169,7 @@
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="90">
-      <c r="A36" s="20" t="s">
+      <c r="A36" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="30">
-      <c r="A37" s="22"/>
+      <c r="A37" s="21"/>
       <c r="B37" s="4" t="s">
         <v>116</v>
       </c>
@@ -2219,7 +2219,7 @@
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="22"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="4" t="s">
         <v>56</v>
       </c>
@@ -2241,7 +2241,7 @@
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8" ht="30">
-      <c r="A39" s="22"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="4" t="s">
         <v>120</v>
       </c>
@@ -2291,7 +2291,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="30">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="16" t="s">
         <v>149</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -2316,38 +2316,15 @@
         <v>125</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="21"/>
-      <c r="B42" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H42" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:H42"/>
-  <mergeCells count="7">
-    <mergeCell ref="A41:A42"/>
+  <autoFilter ref="A1:H41"/>
+  <mergeCells count="6">
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="A13:A16"/>
     <mergeCell ref="A26:A31"/>
     <mergeCell ref="A36:A39"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="A13:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout Upload avatar utilisateur, upload photo présentation spot et action suppression utilisateur
</commit_message>
<xml_diff>
--- a/ActionsStruts.xlsx
+++ b/ActionsStruts.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$43</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="177">
   <si>
     <t>jsp</t>
   </si>
@@ -808,6 +808,27 @@
   </si>
   <si>
     <t>Afficher la liste des exemplaires du topo disponibles aux dates souhaités</t>
+  </si>
+  <si>
+    <t>supprimerExemplaireTopo</t>
+  </si>
+  <si>
+    <t>Supprimer un exemplaire de topo détenu</t>
+  </si>
+  <si>
+    <t>SupprimerExemplaireTopoAction / supprimerExemplaire</t>
+  </si>
+  <si>
+    <t>supprimerUtilisateur</t>
+  </si>
+  <si>
+    <t>Supprimer le compte utilisateur</t>
+  </si>
+  <si>
+    <t>SupprimerUtilisateurAction / supprimer</t>
+  </si>
+  <si>
+    <t>SUCCESS : redirectAction / index</t>
   </si>
 </sst>
 </file>
@@ -958,7 +979,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1005,10 +1026,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,10 +1044,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1320,11 +1347,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="A42:XFD42"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="107" defaultRowHeight="15"/>
@@ -1439,7 +1466,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1463,7 +1490,7 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="22"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1485,7 +1512,7 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="45">
-      <c r="A7" s="22"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -1507,7 +1534,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="22"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -1529,7 +1556,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="22"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1553,7 +1580,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30">
-      <c r="A10" s="22"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1602,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" ht="30">
-      <c r="A11" s="22"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1599,7 +1626,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="22"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1648,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="75">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="18" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1647,7 +1674,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="60">
-      <c r="A14" s="22"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
@@ -1669,7 +1696,7 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8" ht="30">
-      <c r="A15" s="22"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1691,7 +1718,7 @@
       <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:8" ht="30">
-      <c r="A16" s="22"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
@@ -1713,7 +1740,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="1:8" ht="75">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -1739,7 +1766,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30">
-      <c r="A18" s="22"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
@@ -1763,7 +1790,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="90">
-      <c r="A19" s="22"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
@@ -1787,7 +1814,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="30">
-      <c r="A20" s="22"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="4" t="s">
         <v>55</v>
       </c>
@@ -1811,7 +1838,7 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="4" t="s">
         <v>56</v>
       </c>
@@ -1885,7 +1912,7 @@
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -1909,7 +1936,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" ht="30">
-      <c r="A25" s="22"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="15" t="s">
         <v>72</v>
       </c>
@@ -1931,7 +1958,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="19" t="s">
         <v>71</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -1955,7 +1982,7 @@
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="4" t="s">
         <v>75</v>
       </c>
@@ -1979,7 +2006,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="30">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="4" t="s">
         <v>44</v>
       </c>
@@ -2001,7 +2028,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="1:8" ht="45">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="4" t="s">
         <v>155</v>
       </c>
@@ -2025,7 +2052,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="60">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="4" t="s">
         <v>140</v>
       </c>
@@ -2049,7 +2076,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="30">
-      <c r="A31" s="20"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="4" t="s">
         <v>142</v>
       </c>
@@ -2169,7 +2196,7 @@
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8" ht="90">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="22" t="s">
         <v>67</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2195,134 +2222,182 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="30">
-      <c r="A37" s="21"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30">
+      <c r="A38" s="23"/>
+      <c r="B38" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C38" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D38" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E38" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="9" t="s">
+      <c r="F38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="H37" s="9" t="s">
+      <c r="H38" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="21"/>
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:8">
+      <c r="A39" s="23"/>
+      <c r="B39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="E39" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F38" s="5" t="s">
+      <c r="F39" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="1:8" ht="30">
-      <c r="A39" s="21"/>
-      <c r="B39" s="4" t="s">
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" ht="30">
+      <c r="A40" s="23"/>
+      <c r="B40" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E40" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F40" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="60">
-      <c r="A40" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="H40" s="9" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="24"/>
+      <c r="B41" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="60">
+      <c r="A42" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30">
+      <c r="A43" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C43" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E43" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F43" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="G41" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="H41" s="9" t="s">
+      <c r="H43" s="9" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H41"/>
+  <autoFilter ref="A1:H43"/>
   <mergeCells count="6">
+    <mergeCell ref="A36:A41"/>
     <mergeCell ref="A5:A12"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A36:A39"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A17:A21"/>
   </mergeCells>

</xml_diff>